<commit_message>
Semi USB: Checklist: Updating PCB Design Checklist with initial observations and comments for 2_Interface_JTAG
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\2_Interface_JTAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99AAE64-9E46-4F64-9811-917C2C7F38CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A81C9-3DB8-4E9A-AE28-A9B59587787B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3645" windowWidth="29040" windowHeight="15840" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
   <si>
     <t>1.</t>
   </si>
@@ -479,31 +479,46 @@
     <t>Yan Castro de Azeredo</t>
   </si>
   <si>
-    <t>Gabriel Mariano Marcelino</t>
-  </si>
-  <si>
-    <t>Reviewer and Support</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Drawing</t>
   </si>
   <si>
-    <t>André Martins Pio de Mattos</t>
-  </si>
-  <si>
-    <t>USB powered bus</t>
-  </si>
-  <si>
     <t>PCB Design Checklist by Kleber Reis Gouveia Júnior</t>
   </si>
   <si>
     <t>Variant: Semi USB - JTAG Interface Board Nº2</t>
+  </si>
+  <si>
+    <t>Powered from Texas Instruments Debbuger Tool (MSP-FET)</t>
+  </si>
+  <si>
+    <t>Built in MSP-FET</t>
+  </si>
+  <si>
+    <t>No IC used in design</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added template for all schematic sheets </t>
+  </si>
+  <si>
+    <t>Heavy/Taller components must be on top layer</t>
+  </si>
+  <si>
+    <t>Only 2 layers</t>
+  </si>
+  <si>
+    <t>Needed?</t>
+  </si>
+  <si>
+    <t>Waiting more info</t>
+  </si>
+  <si>
+    <t>Needs to be added in specific directory</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1060,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1079,13 +1094,13 @@
         <v>68</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1094,7 +1109,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43949.47189479167</v>
+        <v>43951.835356365744</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1141,7 +1156,7 @@
         <v>133</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1152,7 +1167,9 @@
         <v>78</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="7"/>
     </row>
@@ -1165,8 +1182,12 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7"/>
+      <c r="E8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -1177,8 +1198,12 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="7"/>
+      <c r="E9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -1189,7 +1214,9 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1201,7 +1228,9 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1212,7 +1241,9 @@
         <v>92</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
     </row>
@@ -1225,10 +1256,10 @@
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="7" t="s">
-        <v>151</v>
-      </c>
+      <c r="E13" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -1239,7 +1270,9 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1250,7 +1283,9 @@
         <v>91</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="7"/>
     </row>
@@ -1263,7 +1298,9 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1275,7 +1312,9 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1287,7 +1326,9 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,18 +1340,22 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="7"/>
     </row>
@@ -1318,11 +1363,13 @@
       <c r="A21" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>89</v>
+      <c r="B21" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="7"/>
     </row>
@@ -1331,659 +1378,761 @@
         <v>132</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="15" t="s">
+      <c r="B25" s="24"/>
+      <c r="C25" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D25" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E30" s="2"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="D31" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E31" s="2"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E34" s="2"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E35" s="2"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E37" s="2"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="D39" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E39" s="2"/>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E44" s="2"/>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E45" s="2"/>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E47" s="2"/>
       <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E48" s="2"/>
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E49" s="2"/>
       <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>117</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E53" s="2"/>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E54" s="2"/>
       <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E55" s="2"/>
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E56" s="2"/>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E57" s="2"/>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E58" s="2"/>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E59" s="2"/>
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E60" s="2"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+    <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B62" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="22"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="15" t="s">
+      <c r="B63" s="24"/>
+      <c r="C63" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D63" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E63" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F63" s="15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C64" s="2"/>
-      <c r="D64" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E64" s="2"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C65" s="2"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C66" s="2"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E66" s="2"/>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C67" s="2"/>
-      <c r="D67" s="1"/>
+      <c r="D67" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E67" s="2"/>
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E68" s="2"/>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C69" s="2"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E69" s="2"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C70" s="2"/>
-      <c r="D70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E70" s="2"/>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C71" s="2"/>
-      <c r="D71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+    <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E72" s="2"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B73" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
-      <c r="F72" s="22"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="25" t="s">
+      <c r="B74" s="23"/>
+      <c r="C74" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="26"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="16" t="s">
+      <c r="D74" s="26"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B74" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D74" s="18"/>
-      <c r="E74" s="19"/>
-      <c r="F74" s="14"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>149</v>
@@ -1994,35 +2143,41 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>149</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="17"/>
       <c r="D76" s="18"/>
       <c r="E76" s="19"/>
       <c r="F76" s="14"/>
     </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C74:E74"/>
     <mergeCell ref="C75:E75"/>
     <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A25:B25"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Semi USB: checklist: Updated some itens on PCB Design Checklist schematic section for 2_Interface_JTAG project
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\2_Interface_JTAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A81C9-3DB8-4E9A-AE28-A9B59587787B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71EEE7D-F449-4C21-B909-580B330E9F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="167">
   <si>
     <t>1.</t>
   </si>
@@ -473,9 +473,6 @@
     <t>4.3</t>
   </si>
   <si>
-    <t>Project: Interface Board for FloripaSat-2</t>
-  </si>
-  <si>
     <t>Yan Castro de Azeredo</t>
   </si>
   <si>
@@ -488,9 +485,6 @@
     <t>PCB Design Checklist by Kleber Reis Gouveia Júnior</t>
   </si>
   <si>
-    <t>Variant: Semi USB - JTAG Interface Board Nº2</t>
-  </si>
-  <si>
     <t>Powered from Texas Instruments Debbuger Tool (MSP-FET)</t>
   </si>
   <si>
@@ -519,6 +513,27 @@
   </si>
   <si>
     <t>Needs to be added in specific directory</t>
+  </si>
+  <si>
+    <t>2.37</t>
+  </si>
+  <si>
+    <t>Check the manufacture capabilities for the targeted PBC factory</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>User's guide manual (PDF)</t>
+  </si>
+  <si>
+    <t>Project: Interstage Interface Board for FloripaSat-2</t>
+  </si>
+  <si>
+    <t>Variant: Semi USB - JTAG Interstage Interface Board Nº2</t>
+  </si>
+  <si>
+    <t>Waiting revision</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1075,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1091,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1086,7 +1101,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1094,13 +1109,13 @@
         <v>68</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1109,7 +1124,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43951.835356365744</v>
+        <v>43959.747467592591</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1156,7 +1171,7 @@
         <v>133</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1171,7 +1186,9 @@
         <v>133</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -1186,7 +1203,7 @@
         <v>133</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1202,7 +1219,7 @@
         <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1240,10 +1257,10 @@
       <c r="B12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="7"/>
     </row>
@@ -1282,10 +1299,10 @@
       <c r="B15" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C15" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="7"/>
     </row>
@@ -1350,12 +1367,12 @@
         <v>15</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="7"/>
     </row>
@@ -1380,16 +1397,16 @@
       <c r="B22" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C22" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -1654,7 +1671,7 @@
         <v>133</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,7 +1743,7 @@
         <v>133</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1798,7 +1815,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1814,7 +1831,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1830,7 +1847,7 @@
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1945,56 +1962,56 @@
       <c r="E61" s="2"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B63" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="22"/>
-      <c r="F62" s="22"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="15" t="s">
+      <c r="B64" s="24"/>
+      <c r="C64" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D64" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="E64" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="F64" s="15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="1" t="s">
@@ -2005,10 +2022,10 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="1" t="s">
@@ -2019,10 +2036,10 @@
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="1" t="s">
@@ -2033,10 +2050,10 @@
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="1" t="s">
@@ -2047,10 +2064,10 @@
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="1" t="s">
@@ -2061,10 +2078,10 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="1" t="s">
@@ -2075,10 +2092,10 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="1" t="s">
@@ -2089,10 +2106,10 @@
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="1" t="s">
@@ -2101,83 +2118,111 @@
       <c r="E72" s="2"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
+    <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E73" s="2"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B75" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="23" t="s">
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="23"/>
-      <c r="C74" s="25" t="s">
+      <c r="B76" s="23"/>
+      <c r="C76" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="26"/>
-      <c r="E74" s="27"/>
-      <c r="F74" s="16" t="s">
+      <c r="D76" s="26"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D75" s="18"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="14"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="17"/>
+        <v>135</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>148</v>
+      </c>
       <c r="D77" s="18"/>
       <c r="E77" s="19"/>
       <c r="F77" s="14"/>
     </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="14"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="14"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
     <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B73:F73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="A64:B64"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C76:E76"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Semi USB: checklist: Completed schematic section for PCB Design Checklist for the 2_Interface_JTAG board
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\2_Interface_JTAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71EEE7D-F449-4C21-B909-580B330E9F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0656E8-8BF3-4CBD-9328-DE9590C07146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="172">
   <si>
     <t>1.</t>
   </si>
@@ -534,6 +534,21 @@
   </si>
   <si>
     <t>Waiting revision</t>
+  </si>
+  <si>
+    <t>Power provided from debugger</t>
+  </si>
+  <si>
+    <t>No IC</t>
+  </si>
+  <si>
+    <t>No high speed design</t>
+  </si>
+  <si>
+    <t>Not needed for this specific board</t>
+  </si>
+  <si>
+    <t>Simple PCB design (1 sheet)</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1093,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1139,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43959.747467592591</v>
+        <v>43965.886267824077</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1234,7 +1249,9 @@
       <c r="E10" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -1290,7 +1307,9 @@
       <c r="E14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
@@ -1360,7 +1379,9 @@
       <c r="E19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -1384,11 +1405,13 @@
         <v>94</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="7"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -1412,11 +1435,13 @@
         <v>93</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="7"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">

</xml_diff>

<commit_message>
Semi USB: checklist: Finished PCB Design Checklist for N.2 board close #19
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/2_Interface_JTAG/PCB Design Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\2_Interface_JTAG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0656E8-8BF3-4CBD-9328-DE9590C07146}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717C8D76-0B5D-4FC6-A4E5-040B2156F17A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="188">
   <si>
     <t>1.</t>
   </si>
@@ -500,21 +500,9 @@
     <t xml:space="preserve">Added template for all schematic sheets </t>
   </si>
   <si>
-    <t>Heavy/Taller components must be on top layer</t>
-  </si>
-  <si>
     <t>Only 2 layers</t>
   </si>
   <si>
-    <t>Needed?</t>
-  </si>
-  <si>
-    <t>Waiting more info</t>
-  </si>
-  <si>
-    <t>Needs to be added in specific directory</t>
-  </si>
-  <si>
     <t>2.37</t>
   </si>
   <si>
@@ -527,15 +515,6 @@
     <t>User's guide manual (PDF)</t>
   </si>
   <si>
-    <t>Project: Interstage Interface Board for FloripaSat-2</t>
-  </si>
-  <si>
-    <t>Variant: Semi USB - JTAG Interstage Interface Board Nº2</t>
-  </si>
-  <si>
-    <t>Waiting revision</t>
-  </si>
-  <si>
     <t>Power provided from debugger</t>
   </si>
   <si>
@@ -549,6 +528,75 @@
   </si>
   <si>
     <t>Simple PCB design (1 sheet)</t>
+  </si>
+  <si>
+    <t>Project: Interstage Interface Panels for FloripaSat-2</t>
+  </si>
+  <si>
+    <t>Needing more revision</t>
+  </si>
+  <si>
+    <t>Direct contact opted in power and GND nets</t>
+  </si>
+  <si>
+    <t>Standard 1 oz</t>
+  </si>
+  <si>
+    <t>2 layer 1,6 mm thick</t>
+  </si>
+  <si>
+    <t>Needs revision</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
+    <t>PCB Document mechanical layers configuration and names</t>
+  </si>
+  <si>
+    <t>Gabriel Mariano Marcelino</t>
+  </si>
+  <si>
+    <t>Review and support</t>
+  </si>
+  <si>
+    <t>André Martins de Pio Mattos</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>Edemar Morsch Filho</t>
+  </si>
+  <si>
+    <t>Mechanical validadtion</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>No polarity components</t>
+  </si>
+  <si>
+    <t>Used polygons for power nets</t>
+  </si>
+  <si>
+    <t>0.508 mm to power nets and 0.254 mm to signals</t>
+  </si>
+  <si>
+    <t>Heavy/Taller components must be on top layer for AIT reasons</t>
+  </si>
+  <si>
+    <t>Few components to be an advantage</t>
+  </si>
+  <si>
+    <t>Considering manufacture in JLCPCB</t>
+  </si>
+  <si>
+    <t>Under development</t>
+  </si>
+  <si>
+    <t>Variant: Semi USB - "IIP_RBF" Board Nº2</t>
   </si>
 </sst>
 </file>
@@ -558,7 +606,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-416]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,6 +647,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -691,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -738,6 +805,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1090,10 +1167,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,21 +1182,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="A2" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="7" t="s">
         <v>68</v>
       </c>
@@ -1129,17 +1206,17 @@
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="7" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43965.886267824077</v>
+        <v>44023.953639930558</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1147,19 +1224,19 @@
       <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="15" t="s">
         <v>63</v>
       </c>
@@ -1196,13 +1273,13 @@
       <c r="B7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1250,7 +1327,7 @@
         <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1265,7 +1342,9 @@
       <c r="E11" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -1308,7 +1387,7 @@
         <v>133</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1380,7 +1459,7 @@
         <v>133</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1410,7 +1489,7 @@
         <v>133</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,26 +1519,26 @@
         <v>133</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="24"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="15" t="s">
         <v>63</v>
       </c>
@@ -1485,7 +1564,9 @@
         <v>133</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1494,10 +1575,10 @@
       <c r="B27" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
     </row>
@@ -1509,11 +1590,13 @@
         <v>95</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -1522,10 +1605,10 @@
       <c r="B29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
     </row>
@@ -1536,10 +1619,10 @@
       <c r="B30" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="7"/>
     </row>
@@ -1550,10 +1633,10 @@
       <c r="B31" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="7"/>
     </row>
@@ -1564,10 +1647,10 @@
       <c r="B32" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="7"/>
     </row>
@@ -1578,12 +1661,14 @@
       <c r="B33" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -1593,11 +1678,13 @@
         <v>103</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -1606,10 +1693,10 @@
       <c r="B35" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="7"/>
     </row>
@@ -1620,10 +1707,10 @@
       <c r="B36" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="7"/>
     </row>
@@ -1634,12 +1721,14 @@
       <c r="B37" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -1662,12 +1751,14 @@
       <c r="B39" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -1696,7 +1787,7 @@
         <v>133</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,10 +1797,10 @@
       <c r="B42" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
     </row>
@@ -1734,12 +1825,14 @@
       <c r="B44" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -1748,10 +1841,10 @@
       <c r="B45" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="7"/>
     </row>
@@ -1760,42 +1853,42 @@
         <v>38</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D46" s="2"/>
-      <c r="E46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>156</v>
-      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="7"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="7"/>
     </row>
@@ -1804,12 +1897,12 @@
         <v>41</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="7"/>
     </row>
@@ -1818,13 +1911,13 @@
         <v>42</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,60 +1925,54 @@
         <v>43</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="7" t="s">
-        <v>157</v>
-      </c>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="7" t="s">
-        <v>158</v>
-      </c>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="7" t="s">
-        <v>159</v>
-      </c>
+      <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="7"/>
     </row>
@@ -1894,12 +1981,12 @@
         <v>47</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="7"/>
     </row>
@@ -1908,13 +1995,13 @@
         <v>48</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1922,13 +2009,13 @@
         <v>49</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1936,13 +2023,13 @@
         <v>50</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1950,12 +2037,12 @@
         <v>51</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="7"/>
     </row>
@@ -1964,12 +2051,12 @@
         <v>52</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7"/>
     </row>
@@ -1978,277 +2065,321 @@
         <v>53</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="7"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="D62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B64" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="22"/>
-      <c r="F63" s="22"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="24"/>
-      <c r="C64" s="15" t="s">
+      <c r="B65" s="28"/>
+      <c r="C65" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D65" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E65" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F64" s="15" t="s">
+      <c r="F65" s="15" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="2"/>
       <c r="F66" s="3"/>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="1"/>
       <c r="E67" s="2"/>
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E68" s="2"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="1"/>
       <c r="E69" s="2"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="1"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="1"/>
       <c r="E72" s="2"/>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" s="1"/>
       <c r="E73" s="2"/>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="C74" s="2"/>
-      <c r="D74" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E74" s="2"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F74" s="3"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
+    <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B76" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C75" s="22"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="23" t="s">
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="26"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="23"/>
-      <c r="C76" s="25" t="s">
+      <c r="B77" s="27"/>
+      <c r="C77" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="D76" s="26"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="16" t="s">
+      <c r="D77" s="30"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="16" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D77" s="18"/>
-      <c r="E77" s="19"/>
-      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="19"/>
+        <v>135</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="23"/>
       <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="14"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="17"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="14"/>
+      <c r="B80" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="D80" s="22"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="14"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D81" s="20"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="C77:E77"/>
+  <mergeCells count="16">
+    <mergeCell ref="C81:E81"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C80:E80"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="A65:B65"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>